<commit_message>
Update data package at: 2024-12-03T19:44:34Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_fontes_de_recursos.xlsx
+++ b/data-raw/desc_fontes_de_recursos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1529042\Desktop\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_7BE0024B6A9D680D449A6D16C67FAB0C309AF390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24ED2985-FE84-4041-BD89-A7BFFCF1571B}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_7BE0024B6A9D680D449A6D16C67FAB0C309AF390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4513E470-862C-4940-AC7F-E8625CA6FC9C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,10 +516,10 @@
     <t xml:space="preserve">RECURSOS ADVINDOS DE CONTRIBUIÇÃO PATRONAL, VINCULADOS AO PAGAMENTO DOS BENEFÍCIOS CONCEDIDOS NA FORMA DO ART. 3º DA LEI COMPLEMENTAR Nº 132/2014. </t>
   </si>
   <si>
-    <t>CONTRIBUIÇÃO DO SERVIDOR PARA O FUNPREV</t>
-  </si>
-  <si>
-    <t>RECURSOS ADVINDOS DE CONTRIBUIÇÃO DO SERVIDOR, VINCULADOS AO PAGAMENTO DOS BENEFÍCIOS CONCEDIDOS NA FORMA DO ART. 3º DA LEI COMPLEMENTAR Nº 132/2014.</t>
+    <t>RECURSOS DO ACORDO DE REPACTUAÇÃO DO RIO DOCE</t>
+  </si>
+  <si>
+    <t>RECURSOS PROVENIENTES DO ACORDO JUDICIAL DE REPARAÇÃO INTEGRAL E DEFINITIVA RELATIVA AO ROMPIMENTO DA BARRAGEM DE FUNDÃO EM MARIANA.</t>
   </si>
   <si>
     <t>RECURSOS DE DEPÓSITOS JUDICIAIS - LEI 21.720/15 E LC FEDERAL 151/15</t>
@@ -576,10 +576,10 @@
     <t>RECURSOS PROVENIENTES DA OPERAÇÃO DE SECURITIZAÇÃO DOS ATIVOS DO FUNDO ESPECIAL DE CRÉDITOS INADIMPLIDOS E DÍVIDA ATIVA - FECIDAT, CONFORME ESTABELECIDO NO INCISO II, ARTIGO 34 DA LEI 22.606 DE 20 DE JULHO DE 2017.</t>
   </si>
   <si>
-    <t>RECURSOS DECORRENTES DA COBRANÇA DOS CRÉDITOS INADIMPLIDOS INSCRITOS - LEI 22.606/2017</t>
-  </si>
-  <si>
-    <t>RECURSOS PROVENIENTES DOS CRÉDITOS INADIMPLIDOS INSCRITOS EM DÍVIDA ATIVA OU NÃO, DE NATUREZA TRIBUTÁRIA OU NÃO, QUE ESTEJAM COM PARCELAMENTO EM VIGOR OU NÃO, QUE NÃO ESTEJAM COM EXIGIBILIDADE SUSPENSA E NEM TENHAM SIDO CEDIDOS A MINAS GERAIS PARTICIPAÇÕES S.A. – MGI – INCISO I, ARTIGO 34 DA LEI 22.606/2017.</t>
+    <t>TRANSFERÊNCIAS DO FUNDEB - COMPLEMENTAÇÃO DA UNIÃO - VAAR</t>
+  </si>
+  <si>
+    <t>CONTROLE DOS RECURSOS DE COMPLEMENTAÇÃO DA UNIÃO AO FUNDEB - VAAR, COM BASE NA ALÍNEA C, INCISO V DO ART. 212-A DA CONSTITUIÇÃO FEDERAL.</t>
   </si>
   <si>
     <t>TAXA DE EXPEDIENTE - ADMINISTRAÇÃO INDIRETA</t>
@@ -618,16 +618,16 @@
     <t>RECURSOS PROVENIENTES DA DISTRIBUIÇÃO DOS VALORES ARRECADADOS COM OS LEILÕES DOS VOLUMES EXCEDENTES AO LIMITE A QUE SE REFERE O § 2º DO ART. 1º DA LEI Nº 12.276, DE 30 DE JUNHO DE 2010, AUTORIZADA PELA LEI 13.885 DE 17 DE OUTUBRO DE 2019. OS VALORES SÃO PAGOS A TÍTULO DE BÔNUS DE ASSINATURA PELA EXPLORAÇÃO DO EXCEDENTE DA CESSÃO ONEROSA DO PRÉ-SAL.</t>
   </si>
   <si>
+    <t>TRANSFERÊNCIAS ESPECIAIS DE RECURSOS DA UNIÃO - RECURSOS RECEBIDOS ATÉ 2023</t>
+  </si>
+  <si>
+    <t>RECURSOS TRANSFERIDOS PELA UNIÃO NA FORMA ESTABELECIDA NO INCISO I DO ART.166-A DA CONSTITUIÇÃO DA REPÚBLICA FEDERATIVA DO BRASIL DE 1988. REFERE-SE AOS RECURSOS TRANSFERIDOS PELA UNIÃO AO ESTADO ATÉ O FINAL DO EXERCÍCIO FINANCEIRO DE 2023, BEM COMO A SUAS RESPECTIVAS RESTITUIÇÕES E REMUNERAÇÕES DE DEPÓSITOS BANCÁRIOS, AINDA QUE REGISTRADAS EM EXERCÍCIOS FINANCEIROS POSTERIORES.</t>
+  </si>
+  <si>
     <t>TRANSFERÊNCIAS ESPECIAIS DE RECURSOS DA UNIÃO</t>
   </si>
   <si>
-    <t>RECURSOS TRANSFERIDOS PELA UNIÃO NA FORMA ESTABELECIDA NOS §§ 1º, 2º,3º E 5º DO ART.166-A DA CONSTITUIÇÃO DA REPÚBLICA FEDERATIVA DO BRASIL DE 1988.</t>
-  </si>
-  <si>
-    <t>CONTRIBUIÇÃO MILITAR PARA CUSTEIO DO BENEFÍCIO DE ASSISTÊNCIA À SAÚDE DOS MILITARES E DEPENDENTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTRIBUIÇÃO DESTINADA AO CUSTEIO DO BENEFÍCIO DE ASSISTÊNCIA À SAÚDE DOS MILITARES DA ATIVA, INATIVOS E JUIZ MILITAR DO TRIBUNAL DE JUSTIÇA MILITAR DO ESTADO DE MINAS GERAIS, RESPECTIVOS PENSIONISTAS E DEPENDENTES. </t>
+    <t>RECURSOS TRANSFERIDOS PELA UNIÃO NA FORMA ESTABELECIDA NO INCISO I DO ART.166-A DA CONSTITUIÇÃO DA REPÚBLICA FEDERATIVA DO BRASIL DE 1988. REFERE-SE AOS RECURSOS TRANSFERIDOS PELA UNIÃO AO ESTADO A PARTIR DO EXERCÍCIO FINANCEIRO DE 2024, BEM COMO A SUAS RESPECTIVAS RESTITUIÇÕES E REMUNERAÇÕES DE DEPÓSITOS BANCÁRIOS.</t>
   </si>
   <si>
     <t>AUXÍLIO FINANCEIRO RECEBIDO DA UNIÃO PARA APLICAÇÃO EM AÇÕES DE ENFRENTAMENTO À COVID 19</t>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C100"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.42578125" defaultRowHeight="15"/>
@@ -2074,36 +2074,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName>Sofia Chacon Furletti (SEPLAG)</DisplayName>
-        <AccountId>70</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Rodolfo Pinhón Bechtlufft (SEPLAG)</DisplayName>
-        <AccountId>38</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Carlos Henrique de Oliveira Brochado (SEPLAG)</DisplayName>
-        <AccountId>49</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Carolina Fonseca Moreira (SEPLAG)</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2362,16 +2338,40 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName>Sofia Chacon Furletti (SEPLAG)</DisplayName>
+        <AccountId>70</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rodolfo Pinhón Bechtlufft (SEPLAG)</DisplayName>
+        <AccountId>38</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Carlos Henrique de Oliveira Brochado (SEPLAG)</DisplayName>
+        <AccountId>49</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Carolina Fonseca Moreira (SEPLAG)</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741C4EED-4E68-4D13-8A53-EE95607C61BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52695D42-7905-4355-AFA3-D66DFF9609E9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2379,5 +2379,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52695D42-7905-4355-AFA3-D66DFF9609E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741C4EED-4E68-4D13-8A53-EE95607C61BA}"/>
 </file>
</xml_diff>